<commit_message>
updated some datasheet terms for clarity
</commit_message>
<xml_diff>
--- a/master_count_record.xlsx
+++ b/master_count_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://freshfromflorida-my.sharepoint.com/personal/austin_fife_fdacs_gov/Documents/Documents/rearing_logs/tamarixia_yield/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_1ABD9808A2983EEB99E3471FAC1D38D2F89A00C1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{989FC714-17AD-4710-BFA5-2B275BC8BCCC}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_1ABD9808A2983EEB99E3471FAC1D38D2F89A00C1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE464940-5C75-467E-BE94-57603650EE75}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="3945" windowWidth="21600" windowHeight="12735" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="yield" sheetId="1" r:id="rId1"/>
@@ -97,16 +97,7 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Jasmine</t>
-  </si>
-  <si>
     <t>APHIDS</t>
-  </si>
-  <si>
-    <t>Curry</t>
-  </si>
-  <si>
-    <t>Mix (OJ/Curry)</t>
   </si>
   <si>
     <t>ANTS</t>
@@ -119,6 +110,15 @@
   </si>
   <si>
     <t>Yld</t>
+  </si>
+  <si>
+    <t>M. paniculata</t>
+  </si>
+  <si>
+    <t>B. koenigii</t>
+  </si>
+  <si>
+    <t>Mix</t>
   </si>
 </sst>
 </file>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +680,7 @@
         <v>3</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -748,7 +748,7 @@
         <v>3</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -816,7 +816,7 @@
         <v>3</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -884,7 +884,7 @@
         <v>3</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -952,7 +952,7 @@
         <v>3</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -1020,7 +1020,7 @@
         <v>3</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1088,7 +1088,7 @@
         <v>3</v>
       </c>
       <c r="V8" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1156,7 +1156,7 @@
         <v>3</v>
       </c>
       <c r="V9" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -1224,7 +1224,7 @@
         <v>3</v>
       </c>
       <c r="V10" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -1292,7 +1292,7 @@
         <v>3</v>
       </c>
       <c r="V11" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -1360,7 +1360,7 @@
         <v>3</v>
       </c>
       <c r="V12" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -1428,7 +1428,7 @@
         <v>3</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -1490,13 +1490,13 @@
         <v>0</v>
       </c>
       <c r="T14" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U14" s="7">
         <v>1</v>
       </c>
       <c r="V14" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -1564,7 +1564,7 @@
         <v>1</v>
       </c>
       <c r="V15" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -1626,13 +1626,13 @@
         <v>0</v>
       </c>
       <c r="T16" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U16" s="7">
         <v>1</v>
       </c>
       <c r="V16" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -1700,7 +1700,7 @@
         <v>1</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
@@ -1762,13 +1762,13 @@
         <v>0</v>
       </c>
       <c r="T18" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U18" s="7">
         <v>1</v>
       </c>
       <c r="V18" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
@@ -1836,7 +1836,7 @@
         <v>1</v>
       </c>
       <c r="V19" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
@@ -1898,13 +1898,13 @@
         <v>0</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U20" s="7">
         <v>1</v>
       </c>
       <c r="V20" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
@@ -1966,13 +1966,13 @@
         <v>0</v>
       </c>
       <c r="T21" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U21" s="7">
         <v>1</v>
       </c>
       <c r="V21" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
@@ -2040,7 +2040,7 @@
         <v>1</v>
       </c>
       <c r="V22" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
@@ -2108,7 +2108,7 @@
         <v>1</v>
       </c>
       <c r="V23" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
@@ -2176,7 +2176,7 @@
         <v>1</v>
       </c>
       <c r="V24" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -2244,7 +2244,7 @@
         <v>1</v>
       </c>
       <c r="V25" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -2312,7 +2312,7 @@
         <v>1</v>
       </c>
       <c r="V26" s="7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
@@ -2374,13 +2374,13 @@
         <v>0</v>
       </c>
       <c r="T27" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U27" s="7">
         <v>1</v>
       </c>
       <c r="V27" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
@@ -2448,7 +2448,7 @@
         <v>1</v>
       </c>
       <c r="V28" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
@@ -2516,7 +2516,7 @@
         <v>1</v>
       </c>
       <c r="V29" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
@@ -2584,7 +2584,7 @@
         <v>1</v>
       </c>
       <c r="V30" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
@@ -2652,7 +2652,7 @@
         <v>1</v>
       </c>
       <c r="V31" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
@@ -2720,7 +2720,7 @@
         <v>1</v>
       </c>
       <c r="V32" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
@@ -2782,13 +2782,13 @@
         <v>0</v>
       </c>
       <c r="T33" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U33" s="7">
         <v>1</v>
       </c>
       <c r="V33" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
@@ -2856,7 +2856,7 @@
         <v>1</v>
       </c>
       <c r="V34" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
@@ -2924,7 +2924,7 @@
         <v>1</v>
       </c>
       <c r="V35" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
@@ -2986,13 +2986,13 @@
         <v>0</v>
       </c>
       <c r="T36" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U36" s="7">
         <v>1</v>
       </c>
       <c r="V36" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
@@ -3060,7 +3060,7 @@
         <v>1</v>
       </c>
       <c r="V37" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
@@ -3122,13 +3122,13 @@
         <v>0</v>
       </c>
       <c r="T38" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U38" s="7">
         <v>1</v>
       </c>
       <c r="V38" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
@@ -3196,7 +3196,7 @@
         <v>3</v>
       </c>
       <c r="V39" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
@@ -3264,7 +3264,7 @@
         <v>3</v>
       </c>
       <c r="V40" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
@@ -3332,7 +3332,7 @@
         <v>3</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
@@ -3400,7 +3400,7 @@
         <v>3</v>
       </c>
       <c r="V42" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
@@ -3468,7 +3468,7 @@
         <v>3</v>
       </c>
       <c r="V43" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
@@ -3536,7 +3536,7 @@
         <v>3</v>
       </c>
       <c r="V44" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
@@ -3604,7 +3604,7 @@
         <v>3</v>
       </c>
       <c r="V45" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
@@ -3672,7 +3672,7 @@
         <v>3</v>
       </c>
       <c r="V46" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
@@ -3734,13 +3734,13 @@
         <v>0</v>
       </c>
       <c r="T47" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="U47" s="7">
         <v>3</v>
       </c>
       <c r="V47" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
@@ -3802,13 +3802,13 @@
         <v>0</v>
       </c>
       <c r="T48" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U48" s="7">
         <v>3</v>
       </c>
       <c r="V48" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
@@ -3870,13 +3870,13 @@
         <v>0</v>
       </c>
       <c r="T49" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U49" s="7">
         <v>3</v>
       </c>
       <c r="V49" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
@@ -3938,13 +3938,13 @@
         <v>0</v>
       </c>
       <c r="T50" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U50" s="7">
         <v>3</v>
       </c>
       <c r="V50" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
@@ -4012,7 +4012,7 @@
         <v>3</v>
       </c>
       <c r="V51" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
@@ -4080,7 +4080,7 @@
         <v>3</v>
       </c>
       <c r="V52" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
@@ -4148,7 +4148,7 @@
         <v>3</v>
       </c>
       <c r="V53" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
@@ -4216,7 +4216,7 @@
         <v>3</v>
       </c>
       <c r="V54" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
@@ -4278,13 +4278,13 @@
         <v>0</v>
       </c>
       <c r="T55" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U55" s="7">
         <v>3</v>
       </c>
       <c r="V55" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
@@ -4346,13 +4346,13 @@
         <v>0</v>
       </c>
       <c r="T56" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U56" s="7">
         <v>3</v>
       </c>
       <c r="V56" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
@@ -4414,13 +4414,13 @@
         <v>0</v>
       </c>
       <c r="T57" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U57" s="7">
         <v>3</v>
       </c>
       <c r="V57" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
@@ -4476,7 +4476,7 @@
         <v>1</v>
       </c>
       <c r="V58" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
@@ -4544,7 +4544,7 @@
         <v>1</v>
       </c>
       <c r="V59" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
@@ -4612,7 +4612,7 @@
         <v>1</v>
       </c>
       <c r="V60" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.25">
@@ -4680,7 +4680,7 @@
         <v>1</v>
       </c>
       <c r="V61" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
@@ -4748,7 +4748,7 @@
         <v>1</v>
       </c>
       <c r="V62" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
@@ -4816,7 +4816,7 @@
         <v>1</v>
       </c>
       <c r="V63" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.25">
@@ -4884,7 +4884,7 @@
         <v>1</v>
       </c>
       <c r="V64" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.25">
@@ -4952,7 +4952,7 @@
         <v>1</v>
       </c>
       <c r="V65" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.25">
@@ -5020,7 +5020,7 @@
         <v>1</v>
       </c>
       <c r="V66" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.25">
@@ -5088,7 +5088,7 @@
         <v>1</v>
       </c>
       <c r="V67" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.25">
@@ -5150,7 +5150,7 @@
         <v>1</v>
       </c>
       <c r="V68" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.25">
@@ -5182,7 +5182,7 @@
         <v>1</v>
       </c>
       <c r="V69" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.25">
@@ -5202,7 +5202,7 @@
         <v>1</v>
       </c>
       <c r="V70" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.25">
@@ -5234,7 +5234,7 @@
         <v>1</v>
       </c>
       <c r="V71" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -5290,37 +5290,37 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>15</v>
@@ -5329,10 +5329,10 @@
         <v>16</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>19</v>

</xml_diff>